<commit_message>
GK add links and files to git
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/background_files/מיקום מקורי של הקבצים.xlsx
+++ b/create_forecast_basic/current/background_files/מיקום מקורי של הקבצים.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\creat_forecast_basic\current\background_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3912B58-818B-4024-B7FE-785A2B653B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D972D77B-4F2A-4CEA-8A63-3BD8D18936E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>מספר דירות לפי אזורים סטטיסטיים</t>
   </si>
@@ -282,13 +282,331 @@
   </si>
   <si>
     <t>\\FILE-SRV\Jtmt\projections_team\GIS_backround\INFO\משרד הפנים</t>
+  </si>
+  <si>
+    <t>EMP_kibolet</t>
+  </si>
+  <si>
+    <t>emp_current_year_230718.ipynb</t>
+  </si>
+  <si>
+    <t>\\FILE-SRV\Jtmt\projections_team\תכניות אסטרטגיות לתחבורה ירושלים\תחזיות 2050\תעסוקה\EMP_KIBOLET.gdb</t>
+  </si>
+  <si>
+    <t>\\FILE-SRV\Jtmt\projections_team\GIS_backround\INFO\צתאל\220301_השכלה_גבוהה\סקר_השכלה_גבוהה_2022\out\shp</t>
+  </si>
+  <si>
+    <t>student_dorms.shp</t>
+  </si>
+  <si>
+    <t>commuting_230712.shp</t>
+  </si>
+  <si>
+    <t>\\FILE-SRV\Jtmt\projections_team\תכניות אסטרטגיות לתחבורה ירושלים\תחזיות 2050\תעסוקה</t>
+  </si>
+  <si>
+    <r>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FILE-SRV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tmt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rojections_team</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>כניות אסטרטגיות לתחבורה ירושלים</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>חזיות 2050</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ק</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>בלת מידע</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>תפלגות ענפי כלכלה תעסוקה</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>mp_category_type.shp</t>
+    </r>
+  </si>
+  <si>
+    <t>taz_demo_pls_2020_and_pre_growth_till_2050</t>
+  </si>
+  <si>
+    <r>
+      <t>W:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rojects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>סעת המונים\מטרו</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_שלב ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ק</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>בצי עבודה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>חזיות_דמוגרפיות</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>חזיות_2020</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\מ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>רכיבי_תחזית</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +639,45 @@
       <family val="3"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD7BA7D"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD16969"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD16969"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD7BA7D"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +687,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -338,17 +695,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,18 +807,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:C27" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:C27" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="muni_under_JTMT_ITM"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C32" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6BCCDF95-BDED-4C61-84E1-0F6B5F0AF51D}" name="שם קובץ" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7D45C3C1-4937-4A6F-9B9E-60D2EF57A1C4}" name="מיקום מקורי" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{6288211B-151E-4E12-AEC8-F53A180119A7}" name="קוד בשימוש" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6BCCDF95-BDED-4C61-84E1-0F6B5F0AF51D}" name="שם קובץ" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7D45C3C1-4937-4A6F-9B9E-60D2EF57A1C4}" name="מיקום מקורי" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{6288211B-151E-4E12-AEC8-F53A180119A7}" name="קוד בשימוש" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,21 +1081,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -729,7 +1106,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -740,7 +1117,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -751,7 +1128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -762,7 +1139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -773,7 +1150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -784,7 +1161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -795,7 +1172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -806,7 +1183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -817,7 +1194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -828,7 +1205,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -839,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -850,7 +1227,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -861,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -872,7 +1249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -883,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -894,7 +1271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -905,7 +1282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
@@ -916,7 +1293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -927,7 +1304,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -938,7 +1315,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -949,7 +1326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -960,7 +1337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -971,7 +1348,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -982,7 +1359,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -993,7 +1370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1004,7 +1381,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -1013,6 +1390,61 @@
       </c>
       <c r="C27" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1025,10 +1457,14 @@
     <hyperlink ref="B23" r:id="rId6" xr:uid="{994726E7-02E9-40F1-B829-7A95ADC858C2}"/>
     <hyperlink ref="B24:B25" r:id="rId7" display="\\FILE-SRV\Jtmt\projections_team\GIS_backround\INFO\למ_ס\תלמידים" xr:uid="{4CDE1845-7223-4888-BAC4-3B6721CBFE90}"/>
     <hyperlink ref="B27" r:id="rId8" xr:uid="{81B41BDD-67B3-440A-A369-315E2EA66E75}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{7109532F-634F-40DC-8AF0-A314C8A330B8}"/>
+    <hyperlink ref="B29" r:id="rId10" xr:uid="{5347A49F-8199-4E33-9C67-C6116573389B}"/>
+    <hyperlink ref="B30" r:id="rId11" xr:uid="{B8242891-3EF1-4510-9FFD-A44B5BDEFE6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GK Determining_type_of_age fixed paths
</commit_message>
<xml_diff>
--- a/create_forecast_basic/current/background_files/מיקום מקורי של הקבצים.xlsx
+++ b/create_forecast_basic/current/background_files/מיקום מקורי של הקבצים.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D972D77B-4F2A-4CEA-8A63-3BD8D18936E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE8F47-3869-4726-95C1-00612D2E0C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
   <si>
     <t>מספר דירות לפי אזורים סטטיסטיים</t>
   </si>
@@ -599,6 +599,196 @@
         <scheme val="minor"/>
       </rPr>
       <t>רכיבי_תחזית</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rojects</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>סעת המונים\מטרו</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_שלב ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ק</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>בצי עבודה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>חזיות_דמוגרפיות</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ת</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>חזיות_2050</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ה</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>תפלגות גילים\backround_files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\</t>
+    </r>
+  </si>
+  <si>
+    <t>age_des_types.xlsx</t>
+  </si>
+  <si>
+    <t>Determining_type_of_age_distribution_230719.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AZ_V4_230518_Published.shp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\Model Versions\4.0\TAZ</t>
     </r>
   </si>
 </sst>
@@ -606,7 +796,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +868,12 @@
       <family val="3"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -807,8 +1003,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C32" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C34" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6BCCDF95-BDED-4C61-84E1-0F6B5F0AF51D}" name="שם קובץ" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{7D45C3C1-4937-4A6F-9B9E-60D2EF57A1C4}" name="מיקום מקורי" dataDxfId="1"/>
@@ -1081,21 +1277,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C32"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.8984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1106,7 +1302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1128,7 +1324,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +1335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1150,7 +1346,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1161,7 +1357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1172,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1183,7 +1379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1205,7 +1401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1216,7 +1412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1227,7 +1423,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1238,7 +1434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1249,7 +1445,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1260,7 +1456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1271,7 +1467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1282,7 +1478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>45</v>
       </c>
@@ -1293,7 +1489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1304,7 +1500,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -1315,7 +1511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1326,7 +1522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -1337,7 +1533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -1348,7 +1544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
@@ -1359,7 +1555,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -1370,7 +1566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1381,7 +1577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -1392,7 +1588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
@@ -1403,7 +1599,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>51</v>
       </c>
@@ -1414,7 +1610,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
@@ -1425,7 +1621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>55</v>
       </c>
@@ -1436,7 +1632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>56</v>
       </c>
@@ -1445,6 +1641,28 @@
       </c>
       <c r="C32" s="6" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>